<commit_message>
db.py file will insert data into avani_test-db and test-collection,only BODY,COVER,12T NB,12T WB26T,28T wiil insert all remain will NA
</commit_message>
<xml_diff>
--- a/import/test_gear.xlsx
+++ b/import/test_gear.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\project_3\16-07-2024\project\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00ADB79C-91E1-4068-8B06-49491BC264B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36966CA9-6DF3-4B06-8981-9A0BD9D91C1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{D8515151-6164-46AA-87F0-3D4D4A61D199}"/>
   </bookViews>
@@ -495,7 +495,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -552,7 +552,7 @@
     </row>
     <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11">
-        <v>45450</v>
+        <v>45501</v>
       </c>
       <c r="B2" s="10">
         <v>0</v>

</xml_diff>